<commit_message>
feat: Include color info when importing master dimensions from Excel file Implements #238
</commit_message>
<xml_diff>
--- a/testdata/ctrl-q-master-items.xlsx
+++ b/testdata/ctrl-q-master-items.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goran/parallels_sync/ctrl-q/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goran/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD56630C-38E3-5844-91CD-71C9059123C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E81644A-AFA0-F74A-8918-9C242014764F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{F42C7707-E240-FE44-9311-817D4D57FF24}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <t>Master Item Name</t>
   </si>
@@ -100,15 +100,9 @@
     <t>Country</t>
   </si>
   <si>
-    <t>Geo</t>
-  </si>
-  <si>
     <t>Sales month</t>
   </si>
   <si>
-    <t>Sales calendar</t>
-  </si>
-  <si>
     <t>Month_Sales</t>
   </si>
   <si>
@@ -175,13 +169,81 @@
     <t>='Profit LY'</t>
   </si>
   <si>
-    <t>='Country'</t>
-  </si>
-  <si>
     <t>='Sales month'</t>
   </si>
   <si>
     <t>='Salesperson'</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Per value color</t>
+  </si>
+  <si>
+    <t>{
+    "colors": [
+        {
+            "value": "Afghanistan",
+            "baseColor": {
+                "color": "#8a85c6",
+                "index": -1
+            }
+        },
+        {
+            "value": "Albania",
+            "baseColor": {
+                "color": "#aaaaaa",
+                "index": -1
+            }
+        },
+        {
+            "value": "Algeria",
+            "baseColor": {
+                "color": "#a16090",
+                "index": 9
+            }
+        }
+    ],
+    "nul": {
+        "color": "#c8c7a9",
+        "index": 16
+    },
+    "oth": {
+        "color": "#ffec6e",
+        "index": -1
+    },
+    "pal": null,
+    "single": null,
+    "usePal": true,
+    "autoFill": true
+}</t>
+  </si>
+  <si>
+    <t>Geo, DimCat1</t>
+  </si>
+  <si>
+    <t>='Country sold'</t>
+  </si>
+  <si>
+    <t>{
+  "baseColor": {
+    "color": "#bbbbbb",
+    "index": -1
+  }
+}</t>
+  </si>
+  <si>
+    <t>Color of sold unit</t>
+  </si>
+  <si>
+    <t>='Unit color'</t>
+  </si>
+  <si>
+    <t>Sales, Color</t>
+  </si>
+  <si>
+    <t>UnitColor</t>
   </si>
 </sst>
 </file>
@@ -570,22 +632,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90C8D44-802A-7248-A8B0-E1ADED58E492}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="35.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="31.5" customWidth="1"/>
     <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -602,8 +666,14 @@
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -611,19 +681,19 @@
         <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -631,10 +701,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>10</v>
@@ -643,7 +713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -651,10 +721,10 @@
         <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>9</v>
@@ -663,7 +733,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -671,10 +741,10 @@
         <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>10</v>
@@ -683,7 +753,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -691,10 +761,10 @@
         <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>9</v>
@@ -703,18 +773,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>9</v>
@@ -723,7 +793,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -731,10 +801,10 @@
         <v>14</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>10</v>
@@ -743,7 +813,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" s="3" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -751,56 +821,86 @@
         <v>20</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="G9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="G10" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="3" customFormat="1" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>25</v>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(master-item-import): Include color info when importing master measures from Excel file Implements #245
</commit_message>
<xml_diff>
--- a/testdata/ctrl-q-master-items.xlsx
+++ b/testdata/ctrl-q-master-items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goran/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E81644A-AFA0-F74A-8918-9C242014764F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0445ACF-0681-A540-82D4-F0241F0A327B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{F42C7707-E240-FE44-9311-817D4D57FF24}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
   <si>
     <t>Master Item Name</t>
   </si>
@@ -244,6 +244,45 @@
   </si>
   <si>
     <t>UnitColor</t>
+  </si>
+  <si>
+    <t>{
+  "color": "#8a85c6",
+  "index": 8
+}</t>
+  </si>
+  <si>
+    <t>{
+  "colors": [
+    {
+      "color": "#006580",
+      "index": 6
+    },
+    {
+      "color": "#ac4d58",
+      "index": 10
+    },
+    {
+      "color": "#4477aa",
+      "index": -1
+    },
+    {
+      "color": "#7db8da",
+      "index": -1
+    }
+  ],
+  "breakTypes": [
+    true,
+    true,
+    false
+  ],
+  "limits": [
+    0.223,
+    0.491,
+    0.728
+  ],
+  "limitType": "percent"
+}</t>
   </si>
 </sst>
 </file>
@@ -634,8 +673,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,7 +712,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="188" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -692,8 +731,14 @@
       <c r="F2" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="G2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -712,8 +757,11 @@
       <c r="F3" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="G3" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="190" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -731,6 +779,9 @@
       </c>
       <c r="F4" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat(master-item-import): Add support for importing drill-down dimensions Implements #272
</commit_message>
<xml_diff>
--- a/testdata/ctrl-q-master-items.xlsx
+++ b/testdata/ctrl-q-master-items.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goran/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0445ACF-0681-A540-82D4-F0241F0A327B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56525F3-620B-9941-8EC1-B3C3261F1961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{F42C7707-E240-FE44-9311-817D4D57FF24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sales" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="64">
   <si>
     <t>Master Item Name</t>
   </si>
@@ -284,12 +285,30 @@
   "limitType": "percent"
 }</t>
   </si>
+  <si>
+    <t>dim-drilldown</t>
+  </si>
+  <si>
+    <t>DimDrill</t>
+  </si>
+  <si>
+    <t>Drill-down 1</t>
+  </si>
+  <si>
+    <t>='Drill-down of dimensions'</t>
+  </si>
+  <si>
+    <t>Staff, Color</t>
+  </si>
+  <si>
+    <t>Dim1, Dim2, Dim3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -308,6 +327,20 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -333,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -355,6 +388,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,16 +710,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90C8D44-802A-7248-A8B0-E1ADED58E492}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.33203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="31.5" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
     <col min="6" max="6" width="20.83203125" customWidth="1"/>
     <col min="7" max="7" width="18.6640625" customWidth="1"/>
     <col min="8" max="8" width="23.1640625" customWidth="1"/>
@@ -954,6 +994,29 @@
         <v>55</v>
       </c>
     </row>
+    <row r="13" spans="1:8" ht="90" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>